<commit_message>
edit fault for deploy
</commit_message>
<xml_diff>
--- a/text.xlsx
+++ b/text.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KPY35\Desktop\PYE\anki_th_web_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{779E55B6-885A-4159-A31C-AC76DC321AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCE122C-C67D-4797-A6DA-9088E842FFB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{709CD5AC-28F5-4E1A-B440-37CF72E1A49D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{709CD5AC-28F5-4E1A-B440-37CF72E1A49D}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="home_page" sheetId="4" r:id="rId3"/>
     <sheet name="livereload" sheetId="3" r:id="rId4"/>
     <sheet name="static" sheetId="5" r:id="rId5"/>
+    <sheet name="deploy" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,6 +36,23 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>delete /staticfiles/admin</t>
+  </si>
+  <si>
+    <t>clear all txt (remain only usage file with blank content)</t>
+  </si>
+  <si>
+    <t>put all reference / env folder to same level with manager.py</t>
+  </si>
+  <si>
+    <t>heroku need manager.py on top level</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13642,6 +13660,99 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>204706</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>51785</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39E09F85-AF03-416A-90A9-DC5A668FB751}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="670560" y="175260"/>
+          <a:ext cx="6239746" cy="2505425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>378272</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>40426</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC10389F-67DF-40E9-A942-70FC730AE5B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="670560" y="2979420"/>
+          <a:ext cx="7754432" cy="3019846"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -14089,8 +14200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{824013CA-CD54-4EF9-AC0D-7819523D3718}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -14148,4 +14259,40 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234BD952-047C-46C7-A9F9-193A90281F92}">
+  <dimension ref="B38:B41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetData>
+    <row r="38" spans="2:2">
+      <c r="B38" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
rework frontend, add apkg download
</commit_message>
<xml_diff>
--- a/text.xlsx
+++ b/text.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KPY35\Desktop\PYE\anki_th_web_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37EBD875-3B5E-4B49-877F-33B84E8F0FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A93666-0716-44CE-A135-E9C7F772D7D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{709CD5AC-28F5-4E1A-B440-37CF72E1A49D}"/>
   </bookViews>
@@ -4655,14 +4655,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>385481</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>349622</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>89645</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>268941</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>528917</xdr:colOff>
       <xdr:row>61</xdr:row>
       <xdr:rowOff>170329</xdr:rowOff>
     </xdr:to>
@@ -4679,8 +4679,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1730187" y="9233645"/>
-          <a:ext cx="4589930" cy="1873625"/>
+          <a:off x="1021975" y="9233645"/>
+          <a:ext cx="2868707" cy="1873625"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -8039,16 +8039,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>510985</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>242045</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>108920</xdr:rowOff>
+      <xdr:rowOff>55132</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>376515</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>403413</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>79185</xdr:rowOff>
+      <xdr:rowOff>25397</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -8063,8 +8063,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3200397" y="8535744"/>
-          <a:ext cx="1882589" cy="508147"/>
+          <a:off x="1586751" y="8481956"/>
+          <a:ext cx="1506074" cy="508147"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -10246,6 +10246,209 @@
               </a:solidFill>
             </a:rPr>
             <a:t>apkg</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="2800">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>224119</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>125506</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>89648</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>26896</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="Rectangle: Rounded Corners 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7264A1F8-0643-4011-A9E9-BD0CEA2C1613}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4930590" y="9269506"/>
+          <a:ext cx="537882" cy="1873625"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 2362"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="99FFCC"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="500">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>等</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="500">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>キロ</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="500">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>否</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="500">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>七</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="500">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>四</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>439268</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>37203</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>600636</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>7468</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="Rectangle: Rounded Corners 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D89F37C2-9121-417B-BD2D-B387D4BE62CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4473386" y="8464027"/>
+          <a:ext cx="1506074" cy="508147"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 2362"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="99FFCC"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2800">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Fail</a:t>
           </a:r>
           <a:endParaRPr lang="th-TH" sz="2800">
             <a:solidFill>
@@ -14542,8 +14745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{824013CA-CD54-4EF9-AC0D-7819523D3718}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X35" sqref="X35"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X45" sqref="X45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>